<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI4-Sandbox@47a2175257812e718797ca8a192e101e740cb210 🚀
</commit_message>
<xml_diff>
--- a/all-profiles.xlsx
+++ b/all-profiles.xlsx
@@ -3218,10 +3218,10 @@
     <t>Dosage.maxDosePerLifetime</t>
   </si>
   <si>
-    <t>care-experience-preference</t>
-  </si>
-  <si>
-    <t>http://www.fhir.org/guides/uscdi4-sandbox/StructureDefinition/care-experience-preference</t>
+    <t>us-core-care-experience-preference</t>
+  </si>
+  <si>
+    <t>http://www.fhir.org/guides/uscdi4-sandbox/StructureDefinition/us-core-care-experience-preference</t>
   </si>
   <si>
     <t>USCoreCareExperiencePreferenceProfile</t>

</xml_diff>